<commit_message>
actualizacion a BRE 2.0.1
</commit_message>
<xml_diff>
--- a/src/main/resources/com/relative/brecreditosnuevos/matrices/BaseServicios.xlsx
+++ b/src/main/resources/com/relative/brecreditosnuevos/matrices/BaseServicios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r06xd\Documents\Rogger\Relative\quski-bre\Matrices\Produccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\extre\Documents\proyectos\proyectos drools\quski-bre\Matrices\Matrices v2\Produccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E20E458-B013-4BA7-B902-872F6F2F04E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A1F8C1-3474-4E79-93FC-85592536A3F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9948" yWindow="-36" windowWidth="10548" windowHeight="6828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>RuleSet</t>
   </si>
@@ -169,15 +169,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>0.31,2.0</t>
-  </si>
-  <si>
-    <t>0.31,3.0</t>
-  </si>
-  <si>
-    <t>0.31,4.0</t>
-  </si>
-  <si>
     <t>0.31,6.0</t>
   </si>
   <si>
@@ -190,9 +181,6 @@
     <t>0.31,18.0</t>
   </si>
   <si>
-    <t>0.06,2.0</t>
-  </si>
-  <si>
     <t>0.06,18.0</t>
   </si>
   <si>
@@ -205,12 +193,6 @@
     <t>0.06,6.0</t>
   </si>
   <si>
-    <t>0.06,4.0</t>
-  </si>
-  <si>
-    <t>0.06,3.0</t>
-  </si>
-  <si>
     <t>Variables</t>
   </si>
   <si>
@@ -239,6 +221,27 @@
   </si>
   <si>
     <t xml:space="preserve">SEGURO </t>
+  </si>
+  <si>
+    <t>0.026,2.0</t>
+  </si>
+  <si>
+    <t>0.026,3.0</t>
+  </si>
+  <si>
+    <t>0.026,4.0</t>
+  </si>
+  <si>
+    <t>0.31,7.0</t>
+  </si>
+  <si>
+    <t>0.31,11.0</t>
+  </si>
+  <si>
+    <t>0.06,7.0</t>
+  </si>
+  <si>
+    <t>0.06,11.0</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -430,23 +433,16 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -464,10 +460,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -476,7 +472,6 @@
     <xf numFmtId="2" fontId="6" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -487,7 +482,7 @@
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -503,7 +498,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -799,13 +794,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="12" width="20.77734375" customWidth="1"/>
   </cols>
@@ -825,8 +820,8 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -839,8 +834,8 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -857,404 +852,472 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="L9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="H10" s="16">
+        <v>4.18</v>
+      </c>
+      <c r="I10" s="16">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="H11" s="16">
+        <v>5.25</v>
+      </c>
+      <c r="I11" s="16">
+        <v>1</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="15">
+        <v>4</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="H12" s="16">
+        <v>6.8</v>
+      </c>
+      <c r="I12" s="16">
+        <v>1</v>
+      </c>
+      <c r="J12" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="15">
+        <v>6</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="H13" s="16">
+        <v>10</v>
+      </c>
+      <c r="I13" s="16">
+        <v>1</v>
+      </c>
+      <c r="J13" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="15">
+        <v>7</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="16">
+        <v>7.7</v>
+      </c>
+      <c r="H14" s="16">
+        <v>12.95</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="15">
+        <v>9</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="H15" s="16">
+        <v>12.25</v>
+      </c>
+      <c r="I15" s="16">
+        <v>1</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="15">
+        <v>11</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="16">
+        <v>7.15</v>
+      </c>
+      <c r="H16" s="16">
+        <v>21.45</v>
+      </c>
+      <c r="I16" s="16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="15">
         <v>12</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="E17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="16">
+        <v>3.6</v>
+      </c>
+      <c r="H17" s="16">
+        <v>16</v>
+      </c>
+      <c r="I17" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="15">
         <v>18</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="18">
-        <v>2</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="19">
+      <c r="E18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="16">
         <v>3.6</v>
       </c>
-      <c r="H10" s="19">
-        <v>4.18</v>
-      </c>
-      <c r="I10" s="19">
-        <v>1</v>
-      </c>
-      <c r="J10" s="19">
+      <c r="H18" s="16">
+        <v>19.5</v>
+      </c>
+      <c r="I18" s="16">
         <v>0.5</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-    </row>
-    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="18">
-        <v>3</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="H11" s="19">
-        <v>5.25</v>
-      </c>
-      <c r="I11" s="19">
-        <v>1</v>
-      </c>
-      <c r="J11" s="19">
+      <c r="J18" s="16">
         <v>0.5</v>
       </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-    </row>
-    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="18">
-        <v>4</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="H12" s="19">
-        <v>6.8</v>
-      </c>
-      <c r="I12" s="19">
-        <v>1</v>
-      </c>
-      <c r="J12" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="18">
-        <v>6</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="H13" s="19">
-        <v>10</v>
-      </c>
-      <c r="I13" s="19">
-        <v>1</v>
-      </c>
-      <c r="J13" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="18">
-        <v>9</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="H14" s="19">
-        <v>12.25</v>
-      </c>
-      <c r="I14" s="19">
-        <v>1</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-    </row>
-    <row r="15" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="18">
-        <v>12</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="H15" s="19">
-        <v>16</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="J15" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-    </row>
-    <row r="16" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="18">
-        <v>18</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="H16" s="19">
-        <v>19.5</v>
-      </c>
-      <c r="I16" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="J16" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>